<commit_message>
Removed 2 from run_mh to rerun MH chains
</commit_message>
<xml_diff>
--- a/BIC.xlsx
+++ b/BIC.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\willi\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\willi\Documents\GitHub\Forero_2020\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADC1518F-CBBD-4191-AAF7-2B163424B437}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06B81879-3650-4292-AE91-CC737FB4DD01}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="660" yWindow="480" windowWidth="26955" windowHeight="14115" xr2:uid="{C9F7FF1C-6F61-42FA-AED2-1B9B63B0B133}"/>
+    <workbookView xWindow="135" yWindow="750" windowWidth="22185" windowHeight="14160" xr2:uid="{C9F7FF1C-6F61-42FA-AED2-1B9B63B0B133}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -475,10 +475,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80C0E8BE-B819-43A0-B79F-7470F3384088}">
-  <dimension ref="B1:P32"/>
+  <dimension ref="B1:P35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M34" sqref="M34"/>
+    <sheetView tabSelected="1" topLeftCell="G8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N35" sqref="N35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1293,11 +1293,11 @@
         <v>21</v>
       </c>
       <c r="N30">
-        <f t="shared" ref="N30:P30" si="10" xml:space="preserve"> N31*LOG(8) - 2*-(N29)</f>
+        <f xml:space="preserve"> N31*LOG(8) - 2*-(N29)</f>
         <v>34.540539921951662</v>
       </c>
       <c r="O30">
-        <f t="shared" si="10"/>
+        <f t="shared" ref="N30:P30" si="10" xml:space="preserve"> O31*LOG(8) - 2*-(O29)</f>
         <v>34.534139921951663</v>
       </c>
       <c r="P30">
@@ -1381,6 +1381,20 @@
         <v>39.116199999999999</v>
       </c>
     </row>
+    <row r="35" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N35">
+        <f>N30/2</f>
+        <v>17.270269960975831</v>
+      </c>
+      <c r="O35">
+        <f t="shared" ref="O35:P35" si="13">O30/2</f>
+        <v>17.267069960975832</v>
+      </c>
+      <c r="P35">
+        <f t="shared" si="13"/>
+        <v>16.815824967479859</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="F23:I23 D23">
     <cfRule type="colorScale" priority="24">

</xml_diff>